<commit_message>
add soda tax historical data
</commit_message>
<xml_diff>
--- a/data/01_raw/historical/revenues/Quarterly.xlsx
+++ b/data/01_raw/historical/revenues/Quarterly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/FiveYearPlan/Analysis/five-year-plan-analysis/data/01_raw/historical/revenues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99169B5-17F2-E14C-8535-36CB5D865240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57FC6A1-430B-7246-8121-3157FAD47F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36160" yWindow="1720" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wage &amp; Earnings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="NPT" sheetId="5" r:id="rId5"/>
     <sheet name="Parking" sheetId="6" r:id="rId6"/>
     <sheet name="Amusement" sheetId="7" r:id="rId7"/>
-    <sheet name="Latest Collections Data" sheetId="8" r:id="rId8"/>
+    <sheet name="Soda" sheetId="10" r:id="rId8"/>
+    <sheet name="Latest Collections Data" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
   <si>
     <t>Wage + Earnings History</t>
   </si>
@@ -282,15 +283,34 @@
   <si>
     <t>Amusement</t>
   </si>
+  <si>
+    <t>Soda</t>
+  </si>
+  <si>
+    <t>Soda Tax History</t>
+  </si>
+  <si>
+    <t>May 2021 Revenue Collections Report</t>
+  </si>
+  <si>
+    <t>FYTD Through May</t>
+  </si>
+  <si>
+    <t>May Monthly Total</t>
+  </si>
+  <si>
+    <t>2. "Total" line for last fiscal year should be updated using the audited actual Beverage Tax line in "Supplemental" report.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +456,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -475,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -630,12 +663,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -787,10 +836,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -837,8 +891,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1184,18 +1240,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="79" customWidth="1"/>
-    <col min="2" max="6" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="26" width="15" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.1640625" style="79" customWidth="1"/>
-    <col min="28" max="28" width="8.83203125" style="79" customWidth="1"/>
-    <col min="29" max="29" width="15" style="79" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.5" style="79" customWidth="1"/>
-    <col min="31" max="31" width="21.83203125" style="79" customWidth="1"/>
-    <col min="32" max="38" width="8.83203125" style="79" customWidth="1"/>
-    <col min="39" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="30.33203125" style="80" customWidth="1"/>
+    <col min="2" max="6" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="15" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" style="80" customWidth="1"/>
+    <col min="28" max="28" width="8.83203125" style="80" customWidth="1"/>
+    <col min="29" max="29" width="15" style="80" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.5" style="80" customWidth="1"/>
+    <col min="31" max="31" width="21.83203125" style="80" customWidth="1"/>
+    <col min="32" max="40" width="8.83203125" style="80" customWidth="1"/>
+    <col min="41" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="29" customHeight="1">
@@ -1273,10 +1329,10 @@
       <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:31" ht="21" customHeight="1">
-      <c r="AD4" s="90" t="s">
+      <c r="AD4" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="88"/>
+      <c r="AE4" s="91"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="11" t="s">
@@ -2151,12 +2207,12 @@
       </c>
     </row>
     <row r="17" spans="24:32" ht="21" customHeight="1">
-      <c r="X17" s="92" t="s">
+      <c r="X17" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="93"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="94"/>
+      <c r="Y17" s="96"/>
+      <c r="Z17" s="96"/>
+      <c r="AA17" s="97"/>
       <c r="AD17" s="61" t="s">
         <v>13</v>
       </c>
@@ -2166,19 +2222,19 @@
       </c>
     </row>
     <row r="18" spans="24:32" ht="19" customHeight="1">
-      <c r="X18" s="81" t="s">
+      <c r="X18" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="83"/>
+      <c r="Y18" s="85"/>
+      <c r="Z18" s="85"/>
+      <c r="AA18" s="86"/>
       <c r="AD18" s="61"/>
     </row>
     <row r="19" spans="24:32">
-      <c r="X19" s="84"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
+      <c r="X19" s="87"/>
+      <c r="Y19" s="88"/>
+      <c r="Z19" s="88"/>
+      <c r="AA19" s="89"/>
       <c r="AD19" s="61" t="s">
         <v>19</v>
       </c>
@@ -2188,69 +2244,69 @@
       </c>
     </row>
     <row r="20" spans="24:32" ht="19" customHeight="1">
-      <c r="X20" s="81" t="s">
+      <c r="X20" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
-      <c r="AA20" s="83"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="86"/>
     </row>
     <row r="21" spans="24:32">
-      <c r="X21" s="87"/>
-      <c r="Y21" s="88"/>
-      <c r="Z21" s="88"/>
-      <c r="AA21" s="89"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="91"/>
+      <c r="Z21" s="91"/>
+      <c r="AA21" s="92"/>
     </row>
     <row r="22" spans="24:32" ht="21" customHeight="1">
-      <c r="X22" s="84"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="86"/>
-      <c r="AD22" s="91" t="s">
+      <c r="X22" s="87"/>
+      <c r="Y22" s="88"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="89"/>
+      <c r="AD22" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="AE22" s="88"/>
-      <c r="AF22" s="88"/>
+      <c r="AE22" s="91"/>
+      <c r="AF22" s="91"/>
     </row>
     <row r="23" spans="24:32">
-      <c r="X23" s="81" t="s">
+      <c r="X23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="83"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
+      <c r="AA23" s="86"/>
       <c r="AD23" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="AE23" s="79" t="s">
+      <c r="AE23" s="80" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="24:32">
-      <c r="X24" s="84"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="86"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="88"/>
+      <c r="Z24" s="88"/>
+      <c r="AA24" s="89"/>
     </row>
     <row r="25" spans="24:32" ht="19" customHeight="1">
-      <c r="X25" s="81" t="s">
+      <c r="X25" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="83"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="86"/>
     </row>
     <row r="26" spans="24:32">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:32">
-      <c r="X27" s="84"/>
-      <c r="Y27" s="85"/>
-      <c r="Z27" s="85"/>
-      <c r="AA27" s="86"/>
+      <c r="X27" s="87"/>
+      <c r="Y27" s="88"/>
+      <c r="Z27" s="88"/>
+      <c r="AA27" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2279,13 +2335,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="79" customWidth="1"/>
-    <col min="2" max="5" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.1640625" style="79" customWidth="1"/>
-    <col min="28" max="28" width="13.33203125" style="79" customWidth="1"/>
-    <col min="29" max="35" width="8.83203125" style="79" customWidth="1"/>
-    <col min="36" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="20.5" style="80" customWidth="1"/>
+    <col min="2" max="5" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.1640625" style="80" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" style="80" customWidth="1"/>
+    <col min="29" max="37" width="8.83203125" style="80" customWidth="1"/>
+    <col min="38" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="22" customFormat="1" ht="29" customHeight="1">
@@ -3121,22 +3177,22 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1">
-      <c r="U16" s="96" t="s">
+      <c r="U16" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="V16" s="88"/>
-      <c r="W16" s="88"/>
-      <c r="X16" s="88"/>
-      <c r="Y16" s="88"/>
-      <c r="Z16" s="88"/>
-      <c r="AA16" s="88"/>
-      <c r="AB16" s="88"/>
+      <c r="V16" s="91"/>
+      <c r="W16" s="91"/>
+      <c r="X16" s="91"/>
+      <c r="Y16" s="91"/>
+      <c r="Z16" s="91"/>
+      <c r="AA16" s="91"/>
+      <c r="AB16" s="91"/>
     </row>
     <row r="17" spans="16:28">
-      <c r="R17" s="97" t="s">
+      <c r="R17" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="S17" s="88"/>
+      <c r="S17" s="91"/>
       <c r="V17" s="27" t="s">
         <v>30</v>
       </c>
@@ -3296,12 +3352,12 @@
       <c r="AB22" s="30"/>
     </row>
     <row r="23" spans="16:28" ht="21" customHeight="1">
-      <c r="P23" s="92" t="s">
+      <c r="P23" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="94"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="97"/>
       <c r="U23" t="s">
         <v>45</v>
       </c>
@@ -3326,12 +3382,12 @@
       <c r="AB23" s="30"/>
     </row>
     <row r="24" spans="16:28" ht="19" customHeight="1">
-      <c r="P24" s="81" t="s">
+      <c r="P24" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="Q24" s="82"/>
-      <c r="R24" s="82"/>
-      <c r="S24" s="83"/>
+      <c r="Q24" s="85"/>
+      <c r="R24" s="85"/>
+      <c r="S24" s="86"/>
       <c r="U24" t="s">
         <v>47</v>
       </c>
@@ -3356,10 +3412,10 @@
       <c r="AB24" s="30"/>
     </row>
     <row r="25" spans="16:28">
-      <c r="P25" s="87"/>
-      <c r="Q25" s="88"/>
-      <c r="R25" s="88"/>
-      <c r="S25" s="89"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="91"/>
+      <c r="R25" s="91"/>
+      <c r="S25" s="92"/>
       <c r="U25" t="s">
         <v>48</v>
       </c>
@@ -3384,10 +3440,10 @@
       <c r="AB25" s="30"/>
     </row>
     <row r="26" spans="16:28">
-      <c r="P26" s="87"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="89"/>
+      <c r="P26" s="90"/>
+      <c r="Q26" s="91"/>
+      <c r="R26" s="91"/>
+      <c r="S26" s="92"/>
       <c r="U26" t="s">
         <v>49</v>
       </c>
@@ -3412,10 +3468,10 @@
       <c r="AB26" s="30"/>
     </row>
     <row r="27" spans="16:28">
-      <c r="P27" s="84"/>
-      <c r="Q27" s="85"/>
-      <c r="R27" s="85"/>
-      <c r="S27" s="86"/>
+      <c r="P27" s="87"/>
+      <c r="Q27" s="88"/>
+      <c r="R27" s="88"/>
+      <c r="S27" s="89"/>
       <c r="U27" t="s">
         <v>50</v>
       </c>
@@ -3440,12 +3496,12 @@
       <c r="AB27" s="30"/>
     </row>
     <row r="28" spans="16:28" ht="19" customHeight="1">
-      <c r="P28" s="95" t="s">
+      <c r="P28" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="Q28" s="82"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="83"/>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="86"/>
       <c r="U28" t="s">
         <v>52</v>
       </c>
@@ -3470,10 +3526,10 @@
       <c r="AB28" s="30"/>
     </row>
     <row r="29" spans="16:28">
-      <c r="P29" s="84"/>
-      <c r="Q29" s="85"/>
-      <c r="R29" s="85"/>
-      <c r="S29" s="86"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="88"/>
+      <c r="R29" s="88"/>
+      <c r="S29" s="89"/>
       <c r="U29" t="s">
         <v>53</v>
       </c>
@@ -3498,12 +3554,12 @@
       <c r="AB29" s="33"/>
     </row>
     <row r="30" spans="16:28" ht="19" customHeight="1">
-      <c r="P30" s="95" t="s">
+      <c r="P30" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="Q30" s="82"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="83"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="86"/>
       <c r="U30" s="31" t="s">
         <v>10</v>
       </c>
@@ -3528,10 +3584,10 @@
       <c r="AB30" s="29"/>
     </row>
     <row r="31" spans="16:28" ht="19" customHeight="1">
-      <c r="P31" s="87"/>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="89"/>
+      <c r="P31" s="90"/>
+      <c r="Q31" s="91"/>
+      <c r="R31" s="91"/>
+      <c r="S31" s="92"/>
       <c r="U31" s="32" t="s">
         <v>12</v>
       </c>
@@ -3556,10 +3612,10 @@
       <c r="AB31" s="30"/>
     </row>
     <row r="32" spans="16:28">
-      <c r="P32" s="87"/>
-      <c r="Q32" s="88"/>
-      <c r="R32" s="88"/>
-      <c r="S32" s="89"/>
+      <c r="P32" s="90"/>
+      <c r="Q32" s="91"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="92"/>
       <c r="U32" s="1" t="s">
         <v>14</v>
       </c>
@@ -3584,10 +3640,10 @@
       <c r="AB32" s="30"/>
     </row>
     <row r="33" spans="16:28">
-      <c r="P33" s="84"/>
-      <c r="Q33" s="85"/>
-      <c r="R33" s="85"/>
-      <c r="S33" s="86"/>
+      <c r="P33" s="87"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="88"/>
+      <c r="S33" s="89"/>
       <c r="V33" s="29">
         <v>291045035.30000001</v>
       </c>
@@ -3662,16 +3718,16 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="19.1640625" style="39" customWidth="1"/>
-    <col min="2" max="24" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.83203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.83203125" style="79" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" style="79" customWidth="1"/>
-    <col min="29" max="30" width="8.83203125" style="79" customWidth="1"/>
-    <col min="31" max="31" width="13.5" style="79" customWidth="1"/>
-    <col min="32" max="32" width="18.33203125" style="79" customWidth="1"/>
-    <col min="33" max="39" width="8.83203125" style="79" customWidth="1"/>
-    <col min="40" max="16384" width="8.83203125" style="79"/>
+    <col min="2" max="24" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.83203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.83203125" style="80" customWidth="1"/>
+    <col min="28" max="28" width="9.1640625" style="80" customWidth="1"/>
+    <col min="29" max="30" width="8.83203125" style="80" customWidth="1"/>
+    <col min="31" max="31" width="13.5" style="80" customWidth="1"/>
+    <col min="32" max="32" width="18.33203125" style="80" customWidth="1"/>
+    <col min="33" max="41" width="8.83203125" style="80" customWidth="1"/>
+    <col min="42" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="29" customHeight="1">
@@ -3691,11 +3747,11 @@
     </row>
     <row r="4" spans="1:32" ht="21" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="AD4" s="98" t="s">
+      <c r="AD4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="41"/>
@@ -4556,106 +4612,106 @@
       <c r="AF14" s="69"/>
     </row>
     <row r="15" spans="1:32" ht="21" customHeight="1">
-      <c r="AD15" s="91" t="s">
+      <c r="AD15" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="AE15" s="88"/>
-      <c r="AF15" s="88"/>
+      <c r="AE15" s="91"/>
+      <c r="AF15" s="91"/>
     </row>
     <row r="16" spans="1:32" ht="21" customHeight="1">
-      <c r="X16" s="92" t="s">
+      <c r="X16" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="94"/>
+      <c r="Y16" s="96"/>
+      <c r="Z16" s="96"/>
+      <c r="AA16" s="97"/>
       <c r="AD16" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="AE16" s="79" t="s">
+      <c r="AE16" s="80" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="24:32">
-      <c r="X17" s="81" t="s">
+      <c r="X17" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y17" s="82"/>
-      <c r="Z17" s="82"/>
-      <c r="AA17" s="83"/>
+      <c r="Y17" s="85"/>
+      <c r="Z17" s="85"/>
+      <c r="AA17" s="86"/>
       <c r="AE17" s="61"/>
       <c r="AF17" s="69"/>
     </row>
     <row r="18" spans="24:32" ht="19" customHeight="1">
-      <c r="X18" s="84"/>
-      <c r="Y18" s="85"/>
-      <c r="Z18" s="85"/>
-      <c r="AA18" s="86"/>
+      <c r="X18" s="87"/>
+      <c r="Y18" s="88"/>
+      <c r="Z18" s="88"/>
+      <c r="AA18" s="89"/>
       <c r="AE18" s="61"/>
       <c r="AF18" s="69"/>
     </row>
     <row r="19" spans="24:32">
-      <c r="X19" s="81" t="s">
+      <c r="X19" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="Y19" s="82"/>
-      <c r="Z19" s="82"/>
-      <c r="AA19" s="83"/>
+      <c r="Y19" s="85"/>
+      <c r="Z19" s="85"/>
+      <c r="AA19" s="86"/>
       <c r="AE19" s="61"/>
     </row>
     <row r="20" spans="24:32" ht="19" customHeight="1">
-      <c r="X20" s="87"/>
-      <c r="Y20" s="88"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="89"/>
+      <c r="X20" s="90"/>
+      <c r="Y20" s="91"/>
+      <c r="Z20" s="91"/>
+      <c r="AA20" s="92"/>
       <c r="AE20" s="61"/>
       <c r="AF20" s="69"/>
     </row>
     <row r="21" spans="24:32">
-      <c r="X21" s="84"/>
-      <c r="Y21" s="85"/>
-      <c r="Z21" s="85"/>
-      <c r="AA21" s="86"/>
+      <c r="X21" s="87"/>
+      <c r="Y21" s="88"/>
+      <c r="Z21" s="88"/>
+      <c r="AA21" s="89"/>
     </row>
     <row r="22" spans="24:32">
-      <c r="X22" s="81" t="s">
+      <c r="X22" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y22" s="82"/>
-      <c r="Z22" s="82"/>
-      <c r="AA22" s="83"/>
+      <c r="Y22" s="85"/>
+      <c r="Z22" s="85"/>
+      <c r="AA22" s="86"/>
     </row>
     <row r="23" spans="24:32" ht="19" customHeight="1">
-      <c r="X23" s="84"/>
-      <c r="Y23" s="85"/>
-      <c r="Z23" s="85"/>
-      <c r="AA23" s="86"/>
+      <c r="X23" s="87"/>
+      <c r="Y23" s="88"/>
+      <c r="Z23" s="88"/>
+      <c r="AA23" s="89"/>
     </row>
     <row r="24" spans="24:32">
-      <c r="X24" s="81" t="s">
+      <c r="X24" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y24" s="82"/>
-      <c r="Z24" s="82"/>
-      <c r="AA24" s="83"/>
+      <c r="Y24" s="85"/>
+      <c r="Z24" s="85"/>
+      <c r="AA24" s="86"/>
     </row>
     <row r="25" spans="24:32" ht="19" customHeight="1">
-      <c r="X25" s="87"/>
-      <c r="Y25" s="88"/>
-      <c r="Z25" s="88"/>
-      <c r="AA25" s="89"/>
+      <c r="X25" s="90"/>
+      <c r="Y25" s="91"/>
+      <c r="Z25" s="91"/>
+      <c r="AA25" s="92"/>
     </row>
     <row r="26" spans="24:32">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:32">
-      <c r="X27" s="84"/>
-      <c r="Y27" s="85"/>
-      <c r="Z27" s="85"/>
-      <c r="AA27" s="86"/>
+      <c r="X27" s="87"/>
+      <c r="Y27" s="88"/>
+      <c r="Z27" s="88"/>
+      <c r="AA27" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4684,17 +4740,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="16" style="79" customWidth="1"/>
-    <col min="2" max="8" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="13.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1640625" style="79" customWidth="1"/>
-    <col min="28" max="29" width="8.83203125" style="79" customWidth="1"/>
-    <col min="30" max="30" width="5.83203125" style="79" customWidth="1"/>
-    <col min="31" max="31" width="12.33203125" style="79" customWidth="1"/>
-    <col min="32" max="32" width="8.83203125" style="79" customWidth="1"/>
-    <col min="33" max="33" width="17.83203125" style="79" customWidth="1"/>
-    <col min="34" max="40" width="8.83203125" style="79" customWidth="1"/>
-    <col min="41" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="16" style="80" customWidth="1"/>
+    <col min="2" max="8" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="13.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.1640625" style="80" customWidth="1"/>
+    <col min="28" max="29" width="8.83203125" style="80" customWidth="1"/>
+    <col min="30" max="30" width="5.83203125" style="80" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" style="80" customWidth="1"/>
+    <col min="32" max="32" width="8.83203125" style="80" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" style="80" customWidth="1"/>
+    <col min="34" max="42" width="8.83203125" style="80" customWidth="1"/>
+    <col min="43" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="29" customHeight="1">
@@ -4708,11 +4764,11 @@
       </c>
     </row>
     <row r="4" spans="1:33" ht="21" customHeight="1">
-      <c r="AE4" s="98" t="s">
+      <c r="AE4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
     </row>
     <row r="5" spans="1:33">
       <c r="A5" s="21"/>
@@ -5549,101 +5605,101 @@
       <c r="AA13" s="20">
         <v>299307000</v>
       </c>
-      <c r="AE13" s="91" t="s">
+      <c r="AE13" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="AF13" s="88"/>
-      <c r="AG13" s="88"/>
+      <c r="AF13" s="91"/>
+      <c r="AG13" s="91"/>
     </row>
     <row r="14" spans="1:33">
       <c r="AE14" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AF14" s="79" t="s">
+      <c r="AF14" s="80" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="21" customHeight="1">
-      <c r="X16" s="92" t="s">
+      <c r="X16" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="94"/>
+      <c r="Y16" s="96"/>
+      <c r="Z16" s="96"/>
+      <c r="AA16" s="97"/>
     </row>
     <row r="17" spans="24:27">
-      <c r="X17" s="81" t="s">
+      <c r="X17" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y17" s="82"/>
-      <c r="Z17" s="82"/>
-      <c r="AA17" s="83"/>
+      <c r="Y17" s="85"/>
+      <c r="Z17" s="85"/>
+      <c r="AA17" s="86"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="84"/>
-      <c r="Y18" s="85"/>
-      <c r="Z18" s="85"/>
-      <c r="AA18" s="86"/>
+      <c r="X18" s="87"/>
+      <c r="Y18" s="88"/>
+      <c r="Z18" s="88"/>
+      <c r="AA18" s="89"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="81" t="s">
+      <c r="X19" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="Y19" s="82"/>
-      <c r="Z19" s="82"/>
-      <c r="AA19" s="83"/>
+      <c r="Y19" s="85"/>
+      <c r="Z19" s="85"/>
+      <c r="AA19" s="86"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="87"/>
-      <c r="Y20" s="88"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="89"/>
+      <c r="X20" s="90"/>
+      <c r="Y20" s="91"/>
+      <c r="Z20" s="91"/>
+      <c r="AA20" s="92"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="84"/>
-      <c r="Y21" s="85"/>
-      <c r="Z21" s="85"/>
-      <c r="AA21" s="86"/>
+      <c r="X21" s="87"/>
+      <c r="Y21" s="88"/>
+      <c r="Z21" s="88"/>
+      <c r="AA21" s="89"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="81" t="s">
+      <c r="X22" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y22" s="82"/>
-      <c r="Z22" s="82"/>
-      <c r="AA22" s="83"/>
+      <c r="Y22" s="85"/>
+      <c r="Z22" s="85"/>
+      <c r="AA22" s="86"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="84"/>
-      <c r="Y23" s="85"/>
-      <c r="Z23" s="85"/>
-      <c r="AA23" s="86"/>
+      <c r="X23" s="87"/>
+      <c r="Y23" s="88"/>
+      <c r="Z23" s="88"/>
+      <c r="AA23" s="89"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="81" t="s">
+      <c r="X24" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y24" s="82"/>
-      <c r="Z24" s="82"/>
-      <c r="AA24" s="83"/>
+      <c r="Y24" s="85"/>
+      <c r="Z24" s="85"/>
+      <c r="AA24" s="86"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="87"/>
-      <c r="Y25" s="88"/>
-      <c r="Z25" s="88"/>
-      <c r="AA25" s="89"/>
+      <c r="X25" s="90"/>
+      <c r="Y25" s="91"/>
+      <c r="Z25" s="91"/>
+      <c r="AA25" s="92"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="84"/>
-      <c r="Y27" s="85"/>
-      <c r="Z27" s="85"/>
-      <c r="AA27" s="86"/>
+      <c r="X27" s="87"/>
+      <c r="Y27" s="88"/>
+      <c r="Z27" s="88"/>
+      <c r="AA27" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5672,23 +5728,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="79" customWidth="1"/>
-    <col min="2" max="5" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="79" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="79" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="18" max="25" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" style="79" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" style="79" customWidth="1"/>
-    <col min="28" max="30" width="8.83203125" style="79" customWidth="1"/>
-    <col min="31" max="31" width="11.1640625" style="79" customWidth="1"/>
-    <col min="32" max="32" width="10.33203125" style="79" customWidth="1"/>
-    <col min="33" max="33" width="15" style="79" customWidth="1"/>
-    <col min="34" max="40" width="8.83203125" style="79" customWidth="1"/>
-    <col min="41" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="19.6640625" style="80" customWidth="1"/>
+    <col min="2" max="5" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="80" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="18" max="25" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" style="80" customWidth="1"/>
+    <col min="27" max="27" width="12.83203125" style="80" customWidth="1"/>
+    <col min="28" max="30" width="8.83203125" style="80" customWidth="1"/>
+    <col min="31" max="31" width="11.1640625" style="80" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" style="80" customWidth="1"/>
+    <col min="33" max="33" width="15" style="80" customWidth="1"/>
+    <col min="34" max="42" width="8.83203125" style="80" customWidth="1"/>
+    <col min="43" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="29" customHeight="1">
@@ -5731,12 +5787,12 @@
       <c r="AO3" s="6"/>
     </row>
     <row r="4" spans="1:41" ht="21" customHeight="1">
-      <c r="AD4" s="100" t="s">
+      <c r="AD4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="AM4" s="6"/>
@@ -6670,11 +6726,11 @@
       </c>
     </row>
     <row r="14" spans="1:41" ht="21" customHeight="1">
-      <c r="AE14" s="99" t="s">
+      <c r="AE14" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="AF14" s="88"/>
-      <c r="AG14" s="88"/>
+      <c r="AF14" s="91"/>
+      <c r="AG14" s="91"/>
     </row>
     <row r="15" spans="1:41">
       <c r="AE15" s="52" t="s">
@@ -6686,86 +6742,86 @@
       <c r="AG15" s="6"/>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="92" t="s">
+      <c r="X17" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="93"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="94"/>
+      <c r="Y17" s="96"/>
+      <c r="Z17" s="96"/>
+      <c r="AA17" s="97"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="81" t="s">
+      <c r="X18" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="83"/>
+      <c r="Y18" s="85"/>
+      <c r="Z18" s="85"/>
+      <c r="AA18" s="86"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="84"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
+      <c r="X19" s="87"/>
+      <c r="Y19" s="88"/>
+      <c r="Z19" s="88"/>
+      <c r="AA19" s="89"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="81" t="s">
+      <c r="X20" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
-      <c r="AA20" s="83"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="86"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="87"/>
-      <c r="Y21" s="88"/>
-      <c r="Z21" s="88"/>
-      <c r="AA21" s="89"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="91"/>
+      <c r="Z21" s="91"/>
+      <c r="AA21" s="92"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="84"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="86"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="88"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="89"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="81" t="s">
+      <c r="X23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="83"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
+      <c r="AA23" s="86"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="84"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="86"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="88"/>
+      <c r="Z24" s="88"/>
+      <c r="AA24" s="89"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="81" t="s">
+      <c r="X25" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="83"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="86"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="87"/>
-      <c r="Y27" s="88"/>
-      <c r="Z27" s="88"/>
-      <c r="AA27" s="89"/>
+      <c r="X27" s="90"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91"/>
+      <c r="AA27" s="92"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="84"/>
-      <c r="Y28" s="85"/>
-      <c r="Z28" s="85"/>
-      <c r="AA28" s="86"/>
+      <c r="X28" s="87"/>
+      <c r="Y28" s="88"/>
+      <c r="Z28" s="88"/>
+      <c r="AA28" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6794,14 +6850,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="79" customWidth="1"/>
-    <col min="2" max="23" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="12.83203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.1640625" style="79" customWidth="1"/>
-    <col min="28" max="30" width="12.5" style="79" customWidth="1"/>
-    <col min="31" max="31" width="19.6640625" style="79" customWidth="1"/>
-    <col min="32" max="38" width="8.83203125" style="79" customWidth="1"/>
-    <col min="39" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="28.83203125" style="80" customWidth="1"/>
+    <col min="2" max="23" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12.83203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.1640625" style="80" customWidth="1"/>
+    <col min="28" max="30" width="12.5" style="80" customWidth="1"/>
+    <col min="31" max="31" width="19.6640625" style="80" customWidth="1"/>
+    <col min="32" max="40" width="8.83203125" style="80" customWidth="1"/>
+    <col min="41" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="29" customHeight="1">
@@ -6827,11 +6883,11 @@
       <c r="AK3" s="6"/>
     </row>
     <row r="4" spans="1:37" ht="21" customHeight="1">
-      <c r="AC4" s="100" t="s">
+      <c r="AC4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
+      <c r="AD4" s="91"/>
+      <c r="AE4" s="91"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AK4" s="6"/>
@@ -7726,11 +7782,11 @@
       <c r="AA13" s="56">
         <v>51485000</v>
       </c>
-      <c r="AC13" s="99" t="s">
+      <c r="AC13" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="AD13" s="88"/>
-      <c r="AE13" s="88"/>
+      <c r="AD13" s="91"/>
+      <c r="AE13" s="91"/>
     </row>
     <row r="14" spans="1:37">
       <c r="AC14" s="52" t="s">
@@ -7742,86 +7798,86 @@
       <c r="AE14" s="6"/>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="92" t="s">
+      <c r="X17" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="93"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="94"/>
+      <c r="Y17" s="96"/>
+      <c r="Z17" s="96"/>
+      <c r="AA17" s="97"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="81" t="s">
+      <c r="X18" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="83"/>
+      <c r="Y18" s="85"/>
+      <c r="Z18" s="85"/>
+      <c r="AA18" s="86"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="84"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
+      <c r="X19" s="87"/>
+      <c r="Y19" s="88"/>
+      <c r="Z19" s="88"/>
+      <c r="AA19" s="89"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="81" t="s">
+      <c r="X20" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
-      <c r="AA20" s="83"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="86"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="87"/>
-      <c r="Y21" s="88"/>
-      <c r="Z21" s="88"/>
-      <c r="AA21" s="89"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="91"/>
+      <c r="Z21" s="91"/>
+      <c r="AA21" s="92"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="84"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="86"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="88"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="89"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="81" t="s">
+      <c r="X23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="83"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
+      <c r="AA23" s="86"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="84"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="86"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="88"/>
+      <c r="Z24" s="88"/>
+      <c r="AA24" s="89"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="81" t="s">
+      <c r="X25" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="83"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="86"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="87"/>
-      <c r="Y27" s="88"/>
-      <c r="Z27" s="88"/>
-      <c r="AA27" s="89"/>
+      <c r="X27" s="90"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91"/>
+      <c r="AA27" s="92"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="84"/>
-      <c r="Y28" s="85"/>
-      <c r="Z28" s="85"/>
-      <c r="AA28" s="86"/>
+      <c r="X28" s="87"/>
+      <c r="Y28" s="88"/>
+      <c r="Z28" s="88"/>
+      <c r="AA28" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7844,25 +7900,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="79" customWidth="1"/>
-    <col min="2" max="5" width="11" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="24" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" style="79" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" style="79" customWidth="1"/>
-    <col min="28" max="28" width="8.83203125" style="79" customWidth="1"/>
-    <col min="29" max="29" width="10.33203125" style="79" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="79" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="79" customWidth="1"/>
-    <col min="32" max="32" width="16.1640625" style="79" customWidth="1"/>
-    <col min="33" max="39" width="8.83203125" style="79" customWidth="1"/>
-    <col min="40" max="16384" width="8.83203125" style="79"/>
+    <col min="1" max="1" width="19.5" style="80" customWidth="1"/>
+    <col min="2" max="5" width="11" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="24" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.1640625" style="80" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" style="80" customWidth="1"/>
+    <col min="28" max="28" width="8.83203125" style="80" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" style="80" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" style="80" customWidth="1"/>
+    <col min="31" max="31" width="8.83203125" style="80" customWidth="1"/>
+    <col min="32" max="32" width="16.1640625" style="80" customWidth="1"/>
+    <col min="33" max="41" width="8.83203125" style="80" customWidth="1"/>
+    <col min="42" max="16384" width="8.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="29" customHeight="1">
@@ -7877,11 +7933,11 @@
     </row>
     <row r="4" spans="1:37" ht="21" customHeight="1">
       <c r="A4" s="19"/>
-      <c r="AD4" s="100" t="s">
+      <c r="AD4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
     </row>
@@ -8761,11 +8817,11 @@
       <c r="AA13" s="56">
         <v>2269000</v>
       </c>
-      <c r="AD13" s="99" t="s">
+      <c r="AD13" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="AE13" s="88"/>
-      <c r="AF13" s="88"/>
+      <c r="AE13" s="91"/>
+      <c r="AF13" s="91"/>
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="19"/>
@@ -8778,86 +8834,86 @@
       <c r="AF14" s="6"/>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="92" t="s">
+      <c r="X17" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="93"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="94"/>
+      <c r="Y17" s="96"/>
+      <c r="Z17" s="96"/>
+      <c r="AA17" s="97"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="81" t="s">
+      <c r="X18" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="83"/>
+      <c r="Y18" s="85"/>
+      <c r="Z18" s="85"/>
+      <c r="AA18" s="86"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="84"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
+      <c r="X19" s="87"/>
+      <c r="Y19" s="88"/>
+      <c r="Z19" s="88"/>
+      <c r="AA19" s="89"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="81" t="s">
+      <c r="X20" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
-      <c r="AA20" s="83"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="86"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="87"/>
-      <c r="Y21" s="88"/>
-      <c r="Z21" s="88"/>
-      <c r="AA21" s="89"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="91"/>
+      <c r="Z21" s="91"/>
+      <c r="AA21" s="92"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="84"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="86"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="88"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="89"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="81" t="s">
+      <c r="X23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="83"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
+      <c r="AA23" s="86"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="84"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="86"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="88"/>
+      <c r="Z24" s="88"/>
+      <c r="AA24" s="89"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="81" t="s">
+      <c r="X25" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="83"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="86"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="87"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="92"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="87"/>
-      <c r="Y27" s="88"/>
-      <c r="Z27" s="88"/>
-      <c r="AA27" s="89"/>
+      <c r="X27" s="90"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91"/>
+      <c r="AA27" s="92"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="84"/>
-      <c r="Y28" s="85"/>
-      <c r="Z28" s="85"/>
-      <c r="AA28" s="86"/>
+      <c r="X28" s="87"/>
+      <c r="Y28" s="88"/>
+      <c r="Z28" s="88"/>
+      <c r="AA28" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8877,35 +8933,469 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FD537D-4156-0D46-AC5E-60818D84EF4D}">
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="19.5" style="80" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="80" customWidth="1"/>
+    <col min="3" max="5" width="14.6640625" style="80" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="80" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="80" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="80" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="80" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="80" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="80" customWidth="1"/>
+    <col min="12" max="20" width="8.83203125" style="80" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="29" customHeight="1">
+      <c r="A1" s="48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="24" customHeight="1">
+      <c r="A2" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="21" customHeight="1">
+      <c r="A4" s="19"/>
+      <c r="I4" s="103" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" s="19" customFormat="1">
+      <c r="A5" s="21"/>
+      <c r="B5" s="11">
+        <v>2017</v>
+      </c>
+      <c r="C5" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2020</v>
+      </c>
+      <c r="F5" s="11">
+        <v>2021</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0</v>
+      </c>
+      <c r="C6" s="24">
+        <v>20158107</v>
+      </c>
+      <c r="D6" s="24">
+        <v>20102904</v>
+      </c>
+      <c r="E6" s="24">
+        <v>20280845</v>
+      </c>
+      <c r="F6" s="24">
+        <v>17501595</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0</v>
+      </c>
+      <c r="C7" s="24">
+        <v>19607446</v>
+      </c>
+      <c r="D7" s="24">
+        <v>19254238</v>
+      </c>
+      <c r="E7" s="24">
+        <v>19800740</v>
+      </c>
+      <c r="F7" s="24">
+        <v>17100395</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="70">
+        <f>F13</f>
+        <v>63013000</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="24">
+        <v>12112108</v>
+      </c>
+      <c r="C8" s="24">
+        <v>17826143</v>
+      </c>
+      <c r="D8" s="24">
+        <v>17871411</v>
+      </c>
+      <c r="E8" s="24">
+        <v>17330873</v>
+      </c>
+      <c r="F8" s="24">
+        <v>15075750</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="70">
+        <v>61159657</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="21">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10">
+        <v>20437010</v>
+      </c>
+      <c r="C9" s="10">
+        <v>19698743</v>
+      </c>
+      <c r="D9" s="10">
+        <v>19683380</v>
+      </c>
+      <c r="E9" s="10">
+        <v>13763548</v>
+      </c>
+      <c r="F9" s="18">
+        <f>K11</f>
+        <v>13823121</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="70">
+        <v>5835769</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="25">
+        <f t="shared" ref="B10:F10" si="0">SUM(B6:B9)</f>
+        <v>32549118</v>
+      </c>
+      <c r="C10" s="25">
+        <f t="shared" si="0"/>
+        <v>77290439</v>
+      </c>
+      <c r="D10" s="25">
+        <f t="shared" si="0"/>
+        <v>76911933</v>
+      </c>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
+        <v>71176006</v>
+      </c>
+      <c r="F10" s="25">
+        <f t="shared" si="0"/>
+        <v>63500861</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="K10" s="70">
+        <v>6134009</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="24">
+        <v>0</v>
+      </c>
+      <c r="C11" s="24">
+        <f t="shared" ref="C11:F11" si="1">-B12</f>
+        <v>-6976264.6300000027</v>
+      </c>
+      <c r="D11" s="24">
+        <f t="shared" si="1"/>
+        <v>-7107250.3400000036</v>
+      </c>
+      <c r="E11" s="24">
+        <f t="shared" si="1"/>
+        <v>-7050335.7600000054</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="1"/>
+        <v>-5795135.6400000006</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="70">
+        <f>K7-(K8-K10-K9)</f>
+        <v>13823121</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="24">
+        <f t="shared" ref="B12:F12" si="2">B13-B11-B10</f>
+        <v>6976264.6300000027</v>
+      </c>
+      <c r="C12" s="24">
+        <f t="shared" si="2"/>
+        <v>7107250.3400000036</v>
+      </c>
+      <c r="D12" s="24">
+        <f t="shared" si="2"/>
+        <v>7050335.7600000054</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="2"/>
+        <v>5795135.6400000006</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="2"/>
+        <v>5307274.6400000006</v>
+      </c>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" ht="21" customHeight="1">
+      <c r="A13" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="15">
+        <v>39525382.630000003</v>
+      </c>
+      <c r="C13" s="15">
+        <v>77421424.709999993</v>
+      </c>
+      <c r="D13" s="15">
+        <v>76855018.420000002</v>
+      </c>
+      <c r="E13" s="15">
+        <v>69920805.879999995</v>
+      </c>
+      <c r="F13" s="56">
+        <v>63013000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="21">
+      <c r="A14" s="19"/>
+      <c r="I14" s="102" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="I15" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="17" spans="3:6" ht="21" customHeight="1">
+      <c r="C17" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="97"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="86"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="87"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="89"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="86"/>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="92"/>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="87"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="89"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="86"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="87"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="89"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="86"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="90"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="92"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="90"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="92"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="87"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="89"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C25:F28"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F19"/>
+    <mergeCell ref="C20:F22"/>
+    <mergeCell ref="C23:F24"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{384F67BB-0847-AC46-8F04-F2506C832FAE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50:I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="16" style="79" customWidth="1"/>
-    <col min="2" max="9" width="15.1640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="10.83203125" style="79" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="79"/>
+    <col min="1" max="1" width="16" style="80" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="17" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="10.83203125" style="80" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29" customHeight="1">
       <c r="A1" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="94"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="80" t="s">
         <v>71</v>
       </c>
       <c r="G2" s="76" t="s">
@@ -8914,13 +9404,13 @@
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="G3" s="101" t="s">
+      <c r="G3" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="19" t="s">
@@ -8937,28 +9427,28 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="68"/>
-      <c r="B7" s="80">
+      <c r="B7" s="82">
         <v>2014</v>
       </c>
-      <c r="C7" s="80">
+      <c r="C7" s="82">
         <v>2015</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="82">
         <v>2016</v>
       </c>
-      <c r="E7" s="80">
+      <c r="E7" s="82">
         <v>2017</v>
       </c>
-      <c r="F7" s="80">
+      <c r="F7" s="82">
         <v>2018</v>
       </c>
-      <c r="G7" s="80">
+      <c r="G7" s="82">
         <v>2019</v>
       </c>
-      <c r="H7" s="80">
+      <c r="H7" s="82">
         <v>2020</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9083,28 +9573,28 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="11"/>
-      <c r="B14" s="80">
+      <c r="B14" s="82">
         <v>2014</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="82">
         <v>2015</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="82">
         <v>2016</v>
       </c>
-      <c r="E14" s="80">
+      <c r="E14" s="82">
         <v>2017</v>
       </c>
-      <c r="F14" s="80">
+      <c r="F14" s="82">
         <v>2018</v>
       </c>
-      <c r="G14" s="80">
+      <c r="G14" s="82">
         <v>2019</v>
       </c>
-      <c r="H14" s="80">
+      <c r="H14" s="82">
         <v>2020</v>
       </c>
-      <c r="I14" s="80">
+      <c r="I14" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9229,28 +9719,28 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="11"/>
-      <c r="B21" s="80">
+      <c r="B21" s="82">
         <v>2014</v>
       </c>
-      <c r="C21" s="80">
+      <c r="C21" s="82">
         <v>2015</v>
       </c>
-      <c r="D21" s="80">
+      <c r="D21" s="82">
         <v>2016</v>
       </c>
-      <c r="E21" s="80">
+      <c r="E21" s="82">
         <v>2017</v>
       </c>
-      <c r="F21" s="80">
+      <c r="F21" s="82">
         <v>2018</v>
       </c>
-      <c r="G21" s="80">
+      <c r="G21" s="82">
         <v>2019</v>
       </c>
-      <c r="H21" s="80">
+      <c r="H21" s="82">
         <v>2020</v>
       </c>
-      <c r="I21" s="80">
+      <c r="I21" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9375,28 +9865,28 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="11"/>
-      <c r="B28" s="80">
+      <c r="B28" s="82">
         <v>2014</v>
       </c>
-      <c r="C28" s="80">
+      <c r="C28" s="82">
         <v>2015</v>
       </c>
-      <c r="D28" s="80">
+      <c r="D28" s="82">
         <v>2016</v>
       </c>
-      <c r="E28" s="80">
+      <c r="E28" s="82">
         <v>2017</v>
       </c>
-      <c r="F28" s="80">
+      <c r="F28" s="82">
         <v>2018</v>
       </c>
-      <c r="G28" s="80">
+      <c r="G28" s="82">
         <v>2019</v>
       </c>
-      <c r="H28" s="80">
+      <c r="H28" s="82">
         <v>2020</v>
       </c>
-      <c r="I28" s="80">
+      <c r="I28" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9521,28 +10011,28 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="65"/>
-      <c r="B35" s="80">
+      <c r="B35" s="82">
         <v>2014</v>
       </c>
-      <c r="C35" s="80">
+      <c r="C35" s="82">
         <v>2015</v>
       </c>
-      <c r="D35" s="80">
+      <c r="D35" s="82">
         <v>2016</v>
       </c>
-      <c r="E35" s="80">
+      <c r="E35" s="82">
         <v>2017</v>
       </c>
-      <c r="F35" s="80">
+      <c r="F35" s="82">
         <v>2018</v>
       </c>
-      <c r="G35" s="80">
+      <c r="G35" s="82">
         <v>2019</v>
       </c>
-      <c r="H35" s="80">
+      <c r="H35" s="82">
         <v>2020</v>
       </c>
-      <c r="I35" s="80">
+      <c r="I35" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9667,28 +10157,28 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="65"/>
-      <c r="B42" s="80">
+      <c r="B42" s="82">
         <v>2014</v>
       </c>
-      <c r="C42" s="80">
+      <c r="C42" s="82">
         <v>2015</v>
       </c>
-      <c r="D42" s="80">
+      <c r="D42" s="82">
         <v>2016</v>
       </c>
-      <c r="E42" s="80">
+      <c r="E42" s="82">
         <v>2017</v>
       </c>
-      <c r="F42" s="80">
+      <c r="F42" s="82">
         <v>2018</v>
       </c>
-      <c r="G42" s="80">
+      <c r="G42" s="82">
         <v>2019</v>
       </c>
-      <c r="H42" s="80">
+      <c r="H42" s="82">
         <v>2020</v>
       </c>
-      <c r="I42" s="80">
+      <c r="I42" s="82">
         <v>2021</v>
       </c>
     </row>
@@ -9805,6 +10295,152 @@
         <v>443007</v>
       </c>
       <c r="I46" s="69"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="65"/>
+      <c r="B49" s="79">
+        <v>2014</v>
+      </c>
+      <c r="C49" s="79">
+        <v>2015</v>
+      </c>
+      <c r="D49" s="82">
+        <v>2016</v>
+      </c>
+      <c r="E49" s="82">
+        <v>2017</v>
+      </c>
+      <c r="F49" s="82">
+        <v>2018</v>
+      </c>
+      <c r="G49" s="82">
+        <v>2019</v>
+      </c>
+      <c r="H49" s="82">
+        <v>2020</v>
+      </c>
+      <c r="I49" s="82">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="66">
+        <v>1</v>
+      </c>
+      <c r="B50" s="83">
+        <v>0</v>
+      </c>
+      <c r="C50" s="83">
+        <v>0</v>
+      </c>
+      <c r="D50" s="81">
+        <v>0</v>
+      </c>
+      <c r="E50" s="81">
+        <v>0</v>
+      </c>
+      <c r="F50" s="81">
+        <v>20158107</v>
+      </c>
+      <c r="G50" s="81">
+        <v>20102904</v>
+      </c>
+      <c r="H50" s="81">
+        <v>20280845</v>
+      </c>
+      <c r="I50" s="81">
+        <v>17501595</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="66">
+        <v>2</v>
+      </c>
+      <c r="B51" s="83">
+        <v>0</v>
+      </c>
+      <c r="C51" s="83">
+        <v>0</v>
+      </c>
+      <c r="D51" s="81">
+        <v>0</v>
+      </c>
+      <c r="E51" s="81">
+        <v>0</v>
+      </c>
+      <c r="F51" s="81">
+        <v>19607446</v>
+      </c>
+      <c r="G51" s="81">
+        <v>19254238</v>
+      </c>
+      <c r="H51" s="81">
+        <v>19800740</v>
+      </c>
+      <c r="I51" s="81">
+        <v>17100395</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="66">
+        <v>3</v>
+      </c>
+      <c r="B52" s="83">
+        <v>0</v>
+      </c>
+      <c r="C52" s="83">
+        <v>0</v>
+      </c>
+      <c r="D52" s="81">
+        <v>0</v>
+      </c>
+      <c r="E52" s="81">
+        <v>12112108</v>
+      </c>
+      <c r="F52" s="81">
+        <v>17826143</v>
+      </c>
+      <c r="G52" s="81">
+        <v>17871411</v>
+      </c>
+      <c r="H52" s="81">
+        <v>17330873</v>
+      </c>
+      <c r="I52" s="81">
+        <v>15075750</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="67">
+        <v>4</v>
+      </c>
+      <c r="B53" s="83">
+        <v>0</v>
+      </c>
+      <c r="C53" s="83">
+        <v>0</v>
+      </c>
+      <c r="D53" s="81">
+        <v>0</v>
+      </c>
+      <c r="E53" s="81">
+        <v>20437010</v>
+      </c>
+      <c r="F53" s="81">
+        <v>19698743</v>
+      </c>
+      <c r="G53" s="81">
+        <v>19683380</v>
+      </c>
+      <c r="H53" s="81">
+        <v>13763548</v>
+      </c>
+      <c r="I53" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add final FY24-FY28 forecasts
</commit_message>
<xml_diff>
--- a/data/01_raw/historical/revenues/Quarterly.xlsx
+++ b/data/01_raw/historical/revenues/Quarterly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Analysis/five-year-plan-analysis/data/01_raw/historical/revenues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94213FBD-CC72-C340-8EEB-6EEF984FD51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC6CE39-EEB6-D849-BCC5-5EBC384E8CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wage &amp; Earnings" sheetId="1" r:id="rId1"/>
@@ -862,10 +862,20 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,16 +885,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -893,11 +893,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+    <sheetView topLeftCell="X1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -1351,24 +1351,24 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
-      <c r="AE3" s="90" t="s">
+      <c r="AE3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="89"/>
-      <c r="AH3" s="90" t="s">
+      <c r="AF3" s="95"/>
+      <c r="AH3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="89"/>
+      <c r="AI3" s="95"/>
     </row>
     <row r="4" spans="1:35" ht="21" customHeight="1">
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AH4" s="88" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AH4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="AI4" s="89"/>
+      <c r="AI4" s="95"/>
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="11"/>
@@ -1746,14 +1746,14 @@
       </c>
       <c r="AF8" s="63">
         <f>AC13</f>
-        <v>1703381000</v>
+        <v>1719754000</v>
       </c>
       <c r="AH8" s="55" t="s">
         <v>11</v>
       </c>
       <c r="AI8" s="63">
         <f>AF8</f>
-        <v>1703381000</v>
+        <v>1719754000</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -1843,14 +1843,14 @@
       </c>
       <c r="AC9" s="77">
         <f>AI11</f>
-        <v>380616284</v>
+        <v>396989284</v>
       </c>
       <c r="AE9" s="55" t="s">
         <v>12</v>
       </c>
       <c r="AF9" s="63">
         <f>AF8-AF7</f>
-        <v>842096473</v>
+        <v>858469473</v>
       </c>
       <c r="AH9" s="55" t="s">
         <v>13</v>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="AC10" s="25">
         <f t="shared" si="0"/>
-        <v>1703381000</v>
+        <v>1719754000</v>
       </c>
       <c r="AE10" s="55"/>
       <c r="AF10" s="63"/>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="AI11" s="63">
         <f>AI8-AI9</f>
-        <v>380616284</v>
+        <v>396989284</v>
       </c>
     </row>
     <row r="12" spans="1:35">
@@ -2304,7 +2304,7 @@
         <v>1648127559.5799999</v>
       </c>
       <c r="AC13" s="20">
-        <v>1703381000</v>
+        <v>1719754000</v>
       </c>
       <c r="AE13" s="55"/>
       <c r="AF13" s="78"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="AF14" s="63">
         <f>AF9*AF11</f>
-        <v>446823431.48210317</v>
+        <v>455511082.21835846</v>
       </c>
       <c r="AH14" s="55"/>
       <c r="AI14" s="63"/>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="AF15" s="63">
         <f>AF9*AF12</f>
-        <v>395273041.51789683</v>
+        <v>402958390.78164154</v>
       </c>
       <c r="AH15" s="55"/>
       <c r="AI15" s="63"/>
@@ -2342,71 +2342,71 @@
       <c r="AI16" s="63"/>
     </row>
     <row r="17" spans="24:35" ht="21" customHeight="1">
-      <c r="X17" s="91" t="s">
+      <c r="X17" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="92"/>
-      <c r="AA17" s="93"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="101"/>
       <c r="AE17" s="55"/>
       <c r="AF17" s="63"/>
       <c r="AH17" s="55"/>
       <c r="AI17" s="63"/>
     </row>
     <row r="18" spans="24:35" ht="19" customHeight="1">
-      <c r="X18" s="94" t="s">
+      <c r="X18" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="96"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="90"/>
       <c r="AE18" s="55"/>
       <c r="AF18" s="63"/>
       <c r="AH18" s="55"/>
     </row>
     <row r="19" spans="24:35">
-      <c r="X19" s="99"/>
-      <c r="Y19" s="100"/>
-      <c r="Z19" s="100"/>
-      <c r="AA19" s="101"/>
+      <c r="X19" s="91"/>
+      <c r="Y19" s="92"/>
+      <c r="Z19" s="92"/>
+      <c r="AA19" s="93"/>
       <c r="AE19" s="55"/>
       <c r="AF19" s="63"/>
       <c r="AH19" s="55"/>
       <c r="AI19" s="63"/>
     </row>
     <row r="20" spans="24:35" ht="19" customHeight="1">
-      <c r="X20" s="94" t="s">
+      <c r="X20" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="Y20" s="95"/>
-      <c r="Z20" s="95"/>
-      <c r="AA20" s="96"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="90"/>
       <c r="AE20" s="55"/>
     </row>
     <row r="21" spans="24:35">
-      <c r="X21" s="97"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="98"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="96"/>
       <c r="AE21" s="55"/>
       <c r="AF21" s="63"/>
     </row>
     <row r="22" spans="24:35" ht="21" customHeight="1">
-      <c r="X22" s="99"/>
-      <c r="Y22" s="100"/>
-      <c r="Z22" s="100"/>
-      <c r="AA22" s="101"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="93"/>
       <c r="AH22" s="75" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="24:35">
-      <c r="X23" s="94" t="s">
+      <c r="X23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="95"/>
-      <c r="Z23" s="95"/>
-      <c r="AA23" s="96"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="90"/>
       <c r="AH23" s="55" t="s">
         <v>7</v>
       </c>
@@ -2415,30 +2415,30 @@
       </c>
     </row>
     <row r="24" spans="24:35">
-      <c r="X24" s="99"/>
-      <c r="Y24" s="100"/>
-      <c r="Z24" s="100"/>
-      <c r="AA24" s="101"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="92"/>
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="93"/>
     </row>
     <row r="25" spans="24:35" ht="19" customHeight="1">
-      <c r="X25" s="94" t="s">
+      <c r="X25" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="96"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="90"/>
     </row>
     <row r="26" spans="24:35">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:35" ht="47" customHeight="1">
-      <c r="X27" s="99"/>
-      <c r="Y27" s="100"/>
-      <c r="Z27" s="100"/>
-      <c r="AA27" s="101"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="92"/>
+      <c r="Z27" s="92"/>
+      <c r="AA27" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2466,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView topLeftCell="O2" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView topLeftCell="N3" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -2860,9 +2860,9 @@
         <f>SUM(AB24:AB26)</f>
         <v>98727001.469999984</v>
       </c>
-      <c r="AC8" s="33">
+      <c r="AC8" s="24">
         <f>SUM(AC24:AC26)</f>
-        <v>100529321.44674897</v>
+        <v>103719670</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="AC9" s="18">
         <f>SUM(AC27:AC29)</f>
-        <v>99455740.748337984</v>
+        <v>105357992</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="AC10" s="35">
         <f t="shared" si="0"/>
-        <v>401128101.19508696</v>
+        <v>410220701</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="AC12" s="33">
         <f t="shared" si="2"/>
-        <v>71301449.290299997</v>
+        <v>72491341.361499995</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -3382,26 +3382,26 @@
       </c>
       <c r="AC13" s="34">
         <f t="shared" si="3"/>
-        <v>401602641.48538697</v>
+        <v>411885133.36150002</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="21" customHeight="1">
       <c r="U16" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="V16" s="89"/>
-      <c r="W16" s="89"/>
-      <c r="X16" s="89"/>
-      <c r="Y16" s="89"/>
-      <c r="Z16" s="89"/>
-      <c r="AA16" s="89"/>
-      <c r="AB16" s="89"/>
+      <c r="V16" s="95"/>
+      <c r="W16" s="95"/>
+      <c r="X16" s="95"/>
+      <c r="Y16" s="95"/>
+      <c r="Z16" s="95"/>
+      <c r="AA16" s="95"/>
+      <c r="AB16" s="95"/>
     </row>
     <row r="17" spans="16:30">
       <c r="R17" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="89"/>
+      <c r="S17" s="95"/>
       <c r="V17" s="27" t="s">
         <v>36</v>
       </c>
@@ -3463,8 +3463,7 @@
         <v>35857694</v>
       </c>
       <c r="AD18" s="80">
-        <f>+AC18*1.0067</f>
-        <v>36097940.549800001</v>
+        <v>36700349.809</v>
       </c>
     </row>
     <row r="19" spans="16:30">
@@ -3500,8 +3499,7 @@
         <v>34969215</v>
       </c>
       <c r="AD19" s="80">
-        <f>+AC19*1.0067</f>
-        <v>35203508.740499996</v>
+        <v>35790991.552500002</v>
       </c>
     </row>
     <row r="20" spans="16:30">
@@ -3534,7 +3532,6 @@
         <v>32984118</v>
       </c>
       <c r="AC20" s="81">
-        <f>14923648*2</f>
         <v>29847296</v>
       </c>
     </row>
@@ -3564,7 +3561,6 @@
         <v>30786384</v>
       </c>
       <c r="AC21" s="81">
-        <f>16360012*2</f>
         <v>32720024</v>
       </c>
     </row>
@@ -3594,17 +3590,16 @@
         <v>34645304</v>
       </c>
       <c r="AC22" s="81">
-        <f>17505583*2</f>
         <v>35011166</v>
       </c>
     </row>
     <row r="23" spans="16:30" ht="21" customHeight="1">
-      <c r="P23" s="91" t="s">
+      <c r="P23" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" s="92"/>
-      <c r="R23" s="92"/>
-      <c r="S23" s="93"/>
+      <c r="Q23" s="100"/>
+      <c r="R23" s="100"/>
+      <c r="S23" s="101"/>
       <c r="U23" t="s">
         <v>53</v>
       </c>
@@ -3630,17 +3625,16 @@
         <v>31930512</v>
       </c>
       <c r="AC23" s="81">
-        <f>16368822*2</f>
         <v>32737644</v>
       </c>
     </row>
     <row r="24" spans="16:30" ht="19" customHeight="1">
-      <c r="P24" s="94" t="s">
+      <c r="P24" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="96"/>
+      <c r="Q24" s="89"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="90"/>
       <c r="U24" t="s">
         <v>55</v>
       </c>
@@ -3666,15 +3660,14 @@
         <v>30759393</v>
       </c>
       <c r="AC24" s="81">
-        <f>16053165*2</f>
         <v>32106330</v>
       </c>
     </row>
     <row r="25" spans="16:30">
-      <c r="P25" s="97"/>
-      <c r="Q25" s="89"/>
-      <c r="R25" s="89"/>
-      <c r="S25" s="98"/>
+      <c r="P25" s="94"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="95"/>
+      <c r="S25" s="96"/>
       <c r="U25" t="s">
         <v>56</v>
       </c>
@@ -3700,15 +3693,14 @@
         <v>37155210.229999997</v>
       </c>
       <c r="AC25" s="80">
-        <f>+AB25*1.0067</f>
-        <v>37404150.138540991</v>
+        <v>39470688</v>
       </c>
     </row>
     <row r="26" spans="16:30">
-      <c r="P26" s="97"/>
-      <c r="Q26" s="89"/>
-      <c r="R26" s="89"/>
-      <c r="S26" s="98"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="96"/>
       <c r="U26" t="s">
         <v>57</v>
       </c>
@@ -3734,15 +3726,14 @@
         <v>30812398.239999998</v>
       </c>
       <c r="AC26" s="80">
-        <f>+AB26*1.0067</f>
-        <v>31018841.308207996</v>
+        <v>32142652</v>
       </c>
     </row>
     <row r="27" spans="16:30">
-      <c r="P27" s="99"/>
-      <c r="Q27" s="100"/>
-      <c r="R27" s="100"/>
-      <c r="S27" s="101"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92"/>
+      <c r="S27" s="93"/>
       <c r="U27" t="s">
         <v>58</v>
       </c>
@@ -3768,17 +3759,16 @@
         <v>31367561.079999998</v>
       </c>
       <c r="AC27" s="80">
-        <f>+AB27*1.0067</f>
-        <v>31577723.739235997</v>
+        <v>34484274</v>
       </c>
     </row>
     <row r="28" spans="16:30" ht="19" customHeight="1">
       <c r="P28" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="96"/>
+      <c r="Q28" s="89"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="90"/>
       <c r="U28" t="s">
         <v>60</v>
       </c>
@@ -3804,15 +3794,14 @@
         <v>34542262.130000003</v>
       </c>
       <c r="AC28" s="80">
-        <f>+AB28*1.0067</f>
-        <v>34773695.286270998</v>
+        <v>37210368</v>
       </c>
     </row>
     <row r="29" spans="16:30">
-      <c r="P29" s="99"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
-      <c r="S29" s="101"/>
+      <c r="P29" s="91"/>
+      <c r="Q29" s="92"/>
+      <c r="R29" s="92"/>
+      <c r="S29" s="93"/>
       <c r="U29" t="s">
         <v>61</v>
       </c>
@@ -3838,17 +3827,16 @@
         <v>32883998.93</v>
       </c>
       <c r="AC29" s="80">
-        <f>+AB29*1.0067</f>
-        <v>33104321.722830996</v>
+        <v>33663350</v>
       </c>
     </row>
     <row r="30" spans="16:30" ht="19" customHeight="1">
       <c r="P30" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="95"/>
-      <c r="S30" s="96"/>
+      <c r="Q30" s="89"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="90"/>
       <c r="U30" s="31" t="s">
         <v>14</v>
       </c>
@@ -3874,14 +3862,14 @@
         <v>393809088.61000001</v>
       </c>
       <c r="AC30" s="29">
-        <v>401128101.19508702</v>
+        <v>410220701</v>
       </c>
     </row>
     <row r="31" spans="16:30" ht="19" customHeight="1">
-      <c r="P31" s="97"/>
-      <c r="Q31" s="89"/>
-      <c r="R31" s="89"/>
-      <c r="S31" s="98"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="96"/>
       <c r="U31" s="32" t="s">
         <v>16</v>
       </c>
@@ -3911,10 +3899,10 @@
       </c>
     </row>
     <row r="32" spans="16:30">
-      <c r="P32" s="97"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="98"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="96"/>
       <c r="U32" s="1" t="s">
         <v>19</v>
       </c>
@@ -3940,14 +3928,14 @@
         <v>70826909</v>
       </c>
       <c r="AC32" s="30">
-        <v>71301449.290299997</v>
+        <v>72491341.361499995</v>
       </c>
     </row>
     <row r="33" spans="16:29">
-      <c r="P33" s="99"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="100"/>
-      <c r="S33" s="101"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="92"/>
+      <c r="R33" s="92"/>
+      <c r="S33" s="93"/>
       <c r="V33" s="29">
         <v>291045035.30000001</v>
       </c>
@@ -3970,7 +3958,7 @@
         <v>398694050.61000001</v>
       </c>
       <c r="AC33" s="29">
-        <v>401602641.48538703</v>
+        <v>411885133.36150002</v>
       </c>
     </row>
     <row r="34" spans="16:29">
@@ -4022,7 +4010,7 @@
   <dimension ref="A1:AJ27"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -4058,27 +4046,27 @@
       <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="90" t="s">
+      <c r="AE3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="89"/>
-      <c r="AH3" s="90" t="s">
+      <c r="AF3" s="95"/>
+      <c r="AH3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="89"/>
-      <c r="AJ3" s="89"/>
+      <c r="AI3" s="95"/>
+      <c r="AJ3" s="95"/>
     </row>
     <row r="4" spans="1:36" ht="21" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AH4" s="106" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AH4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="89"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="38"/>
@@ -4454,14 +4442,14 @@
       </c>
       <c r="AF8" s="63">
         <f>AC13</f>
-        <v>729455000</v>
+        <v>690754000</v>
       </c>
       <c r="AI8" s="55" t="s">
         <v>11</v>
       </c>
       <c r="AJ8" s="63">
         <f>AC13</f>
-        <v>729455000</v>
+        <v>690754000</v>
       </c>
     </row>
     <row r="9" spans="1:36">
@@ -4551,14 +4539,14 @@
       </c>
       <c r="AC9" s="18">
         <f>AF15</f>
-        <v>495078014.08938205</v>
+        <v>462106729.07634795</v>
       </c>
       <c r="AE9" s="55" t="s">
         <v>12</v>
       </c>
       <c r="AF9" s="63">
         <f>AF8-AF7</f>
-        <v>581112147</v>
+        <v>542411147</v>
       </c>
       <c r="AI9" s="55" t="s">
         <v>66</v>
@@ -4679,7 +4667,7 @@
       </c>
       <c r="AC10" s="25">
         <f t="shared" si="0"/>
-        <v>722369795.08938205</v>
+        <v>689398510.07634795</v>
       </c>
       <c r="AE10" s="55"/>
       <c r="AF10" s="63"/>
@@ -4796,7 +4784,7 @@
       </c>
       <c r="AJ11" s="63">
         <f>AJ8-(AJ9-AJ10)</f>
-        <v>729455000</v>
+        <v>690754000</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -4893,7 +4881,7 @@
       </c>
       <c r="AC12" s="24">
         <f t="shared" si="2"/>
-        <v>12670966.500617981</v>
+        <v>6941251.5136520863</v>
       </c>
       <c r="AE12" s="55" t="s">
         <v>20</v>
@@ -5009,7 +4997,7 @@
         <v>749865139.25999999</v>
       </c>
       <c r="AC13" s="20">
-        <v>729455000</v>
+        <v>690754000</v>
       </c>
       <c r="AE13" s="55"/>
       <c r="AF13" s="78"/>
@@ -5023,13 +5011,13 @@
       </c>
       <c r="AF14" s="63">
         <f>AF9*AF11</f>
-        <v>86034132.910617962</v>
-      </c>
-      <c r="AH14" s="105" t="s">
+        <v>80304417.923652068</v>
+      </c>
+      <c r="AH14" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="AI14" s="89"/>
-      <c r="AJ14" s="89"/>
+      <c r="AI14" s="95"/>
+      <c r="AJ14" s="95"/>
     </row>
     <row r="15" spans="1:36" ht="21" customHeight="1">
       <c r="AE15" s="55" t="s">
@@ -5037,7 +5025,7 @@
       </c>
       <c r="AF15" s="63">
         <f>AF9*AF12</f>
-        <v>495078014.08938205</v>
+        <v>462106729.07634795</v>
       </c>
       <c r="AH15" s="55" t="s">
         <v>7</v>
@@ -5047,94 +5035,94 @@
       </c>
     </row>
     <row r="16" spans="1:36" ht="21" customHeight="1">
-      <c r="X16" s="91" t="s">
+      <c r="X16" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y16" s="92"/>
-      <c r="Z16" s="92"/>
-      <c r="AA16" s="93"/>
+      <c r="Y16" s="100"/>
+      <c r="Z16" s="100"/>
+      <c r="AA16" s="101"/>
     </row>
     <row r="17" spans="24:33">
-      <c r="X17" s="94" t="s">
+      <c r="X17" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y17" s="95"/>
-      <c r="Z17" s="95"/>
-      <c r="AA17" s="96"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="90"/>
       <c r="AE17" s="55"/>
       <c r="AF17" s="63"/>
       <c r="AG17" s="63"/>
     </row>
     <row r="18" spans="24:33" ht="19" customHeight="1">
-      <c r="X18" s="99"/>
-      <c r="Y18" s="100"/>
-      <c r="Z18" s="100"/>
-      <c r="AA18" s="101"/>
+      <c r="X18" s="91"/>
+      <c r="Y18" s="92"/>
+      <c r="Z18" s="92"/>
+      <c r="AA18" s="93"/>
       <c r="AF18" s="55"/>
       <c r="AG18" s="63"/>
     </row>
     <row r="19" spans="24:33">
-      <c r="X19" s="94" t="s">
+      <c r="X19" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="Y19" s="95"/>
-      <c r="Z19" s="95"/>
-      <c r="AA19" s="96"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="90"/>
       <c r="AF19" s="55"/>
     </row>
     <row r="20" spans="24:33" ht="19" customHeight="1">
-      <c r="X20" s="97"/>
-      <c r="Y20" s="89"/>
-      <c r="Z20" s="89"/>
-      <c r="AA20" s="98"/>
+      <c r="X20" s="94"/>
+      <c r="Y20" s="95"/>
+      <c r="Z20" s="95"/>
+      <c r="AA20" s="96"/>
       <c r="AF20" s="55"/>
       <c r="AG20" s="63"/>
     </row>
     <row r="21" spans="24:33">
-      <c r="X21" s="99"/>
-      <c r="Y21" s="100"/>
-      <c r="Z21" s="100"/>
-      <c r="AA21" s="101"/>
+      <c r="X21" s="91"/>
+      <c r="Y21" s="92"/>
+      <c r="Z21" s="92"/>
+      <c r="AA21" s="93"/>
     </row>
     <row r="22" spans="24:33">
-      <c r="X22" s="94" t="s">
+      <c r="X22" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" s="95"/>
-      <c r="Z22" s="95"/>
-      <c r="AA22" s="96"/>
+      <c r="Y22" s="89"/>
+      <c r="Z22" s="89"/>
+      <c r="AA22" s="90"/>
     </row>
     <row r="23" spans="24:33" ht="19" customHeight="1">
-      <c r="X23" s="99"/>
-      <c r="Y23" s="100"/>
-      <c r="Z23" s="100"/>
-      <c r="AA23" s="101"/>
+      <c r="X23" s="91"/>
+      <c r="Y23" s="92"/>
+      <c r="Z23" s="92"/>
+      <c r="AA23" s="93"/>
     </row>
     <row r="24" spans="24:33">
-      <c r="X24" s="94" t="s">
+      <c r="X24" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="Y24" s="95"/>
-      <c r="Z24" s="95"/>
-      <c r="AA24" s="96"/>
+      <c r="Y24" s="89"/>
+      <c r="Z24" s="89"/>
+      <c r="AA24" s="90"/>
     </row>
     <row r="25" spans="24:33" ht="19" customHeight="1">
-      <c r="X25" s="97"/>
-      <c r="Y25" s="89"/>
-      <c r="Z25" s="89"/>
-      <c r="AA25" s="98"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="95"/>
+      <c r="Z25" s="95"/>
+      <c r="AA25" s="96"/>
     </row>
     <row r="26" spans="24:33">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:33">
-      <c r="X27" s="99"/>
-      <c r="Y27" s="100"/>
-      <c r="Z27" s="100"/>
-      <c r="AA27" s="101"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="92"/>
+      <c r="Z27" s="92"/>
+      <c r="AA27" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5159,7 +5147,7 @@
   <dimension ref="A1:AK27"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+      <selection activeCell="AK9" sqref="AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -5192,26 +5180,26 @@
       </c>
     </row>
     <row r="3" spans="1:37">
-      <c r="AE3" s="90" t="s">
+      <c r="AE3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="89"/>
-      <c r="AI3" s="90" t="s">
+      <c r="AF3" s="95"/>
+      <c r="AI3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="89"/>
-      <c r="AK3" s="89"/>
+      <c r="AJ3" s="95"/>
+      <c r="AK3" s="95"/>
     </row>
     <row r="4" spans="1:37" ht="21" customHeight="1">
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AI4" s="106" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AI4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="21"/>
@@ -5587,13 +5575,13 @@
       </c>
       <c r="AF8" s="63">
         <f>AC13</f>
-        <v>398824000</v>
+        <v>381304000</v>
       </c>
       <c r="AJ8" s="55" t="s">
         <v>11</v>
       </c>
       <c r="AK8" s="63">
-        <v>398824000</v>
+        <v>381304000</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -5683,14 +5671,14 @@
       </c>
       <c r="AC9" s="18">
         <f>AK10</f>
-        <v>89237193</v>
+        <v>71717193</v>
       </c>
       <c r="AE9" s="55" t="s">
         <v>12</v>
       </c>
       <c r="AF9" s="63">
         <f>AF8-AF7</f>
-        <v>152546960</v>
+        <v>135026960</v>
       </c>
       <c r="AJ9" s="55" t="s">
         <v>71</v>
@@ -5814,7 +5802,7 @@
       </c>
       <c r="AC10" s="25">
         <f t="shared" si="0"/>
-        <v>398824000</v>
+        <v>381304000</v>
       </c>
       <c r="AE10" s="55"/>
       <c r="AF10" s="63"/>
@@ -5823,7 +5811,7 @@
       </c>
       <c r="AK10" s="63">
         <f>AK8-AK9</f>
-        <v>89237193</v>
+        <v>71717193</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -6143,15 +6131,15 @@
       </c>
       <c r="AC13" s="20">
         <f>AK8</f>
-        <v>398824000</v>
+        <v>381304000</v>
       </c>
       <c r="AE13" s="55"/>
       <c r="AF13" s="78"/>
-      <c r="AI13" s="105" t="s">
+      <c r="AI13" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="AJ13" s="89"/>
-      <c r="AK13" s="89"/>
+      <c r="AJ13" s="95"/>
+      <c r="AK13" s="95"/>
     </row>
     <row r="14" spans="1:37" ht="21" customHeight="1">
       <c r="AE14" s="55" t="s">
@@ -6159,7 +6147,7 @@
       </c>
       <c r="AF14" s="63">
         <f>AF9*AF11</f>
-        <v>83158061.001093581</v>
+        <v>73607367.701540709</v>
       </c>
       <c r="AI14" s="55" t="s">
         <v>7</v>
@@ -6174,90 +6162,90 @@
       </c>
       <c r="AF15" s="63">
         <f>AF9*AF12</f>
-        <v>69388898.998906419</v>
+        <v>61419592.298459284</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="21" customHeight="1">
-      <c r="X16" s="91" t="s">
+      <c r="X16" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y16" s="92"/>
-      <c r="Z16" s="92"/>
-      <c r="AA16" s="93"/>
+      <c r="Y16" s="100"/>
+      <c r="Z16" s="100"/>
+      <c r="AA16" s="101"/>
     </row>
     <row r="17" spans="24:27">
-      <c r="X17" s="94" t="s">
+      <c r="X17" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y17" s="95"/>
-      <c r="Z17" s="95"/>
-      <c r="AA17" s="96"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="90"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="99"/>
-      <c r="Y18" s="100"/>
-      <c r="Z18" s="100"/>
-      <c r="AA18" s="101"/>
+      <c r="X18" s="91"/>
+      <c r="Y18" s="92"/>
+      <c r="Z18" s="92"/>
+      <c r="AA18" s="93"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="94" t="s">
+      <c r="X19" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="Y19" s="95"/>
-      <c r="Z19" s="95"/>
-      <c r="AA19" s="96"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="90"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="97"/>
-      <c r="Y20" s="89"/>
-      <c r="Z20" s="89"/>
-      <c r="AA20" s="98"/>
+      <c r="X20" s="94"/>
+      <c r="Y20" s="95"/>
+      <c r="Z20" s="95"/>
+      <c r="AA20" s="96"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="99"/>
-      <c r="Y21" s="100"/>
-      <c r="Z21" s="100"/>
-      <c r="AA21" s="101"/>
+      <c r="X21" s="91"/>
+      <c r="Y21" s="92"/>
+      <c r="Z21" s="92"/>
+      <c r="AA21" s="93"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="94" t="s">
+      <c r="X22" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" s="95"/>
-      <c r="Z22" s="95"/>
-      <c r="AA22" s="96"/>
+      <c r="Y22" s="89"/>
+      <c r="Z22" s="89"/>
+      <c r="AA22" s="90"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="99"/>
-      <c r="Y23" s="100"/>
-      <c r="Z23" s="100"/>
-      <c r="AA23" s="101"/>
+      <c r="X23" s="91"/>
+      <c r="Y23" s="92"/>
+      <c r="Z23" s="92"/>
+      <c r="AA23" s="93"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="94" t="s">
+      <c r="X24" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="Y24" s="95"/>
-      <c r="Z24" s="95"/>
-      <c r="AA24" s="96"/>
+      <c r="Y24" s="89"/>
+      <c r="Z24" s="89"/>
+      <c r="AA24" s="90"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="97"/>
-      <c r="Y25" s="89"/>
-      <c r="Z25" s="89"/>
-      <c r="AA25" s="98"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="95"/>
+      <c r="Z25" s="95"/>
+      <c r="AA25" s="96"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="99"/>
-      <c r="Y27" s="100"/>
-      <c r="Z27" s="100"/>
-      <c r="AA27" s="101"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="92"/>
+      <c r="Z27" s="92"/>
+      <c r="AA27" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -6282,7 +6270,7 @@
   <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -6339,15 +6327,15 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:37" ht="21" customHeight="1">
-      <c r="AE4" s="90" t="s">
+      <c r="AE4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AI4" s="90" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AI4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
     </row>
     <row r="5" spans="1:37" ht="21" customHeight="1">
       <c r="A5" s="21"/>
@@ -6435,15 +6423,15 @@
       <c r="AC5" s="11">
         <v>2023</v>
       </c>
-      <c r="AE5" s="88" t="s">
+      <c r="AE5" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AF5" s="89"/>
-      <c r="AI5" s="106" t="s">
+      <c r="AF5" s="95"/>
+      <c r="AI5" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="AJ5" s="89"/>
-      <c r="AK5" s="89"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="9">
@@ -6813,21 +6801,21 @@
       </c>
       <c r="AC9" s="33">
         <f>AF16</f>
-        <v>17530845.89622917</v>
+        <v>27154761.818224419</v>
       </c>
       <c r="AE9" s="55" t="s">
         <v>10</v>
       </c>
       <c r="AF9" s="63">
         <f>AC13</f>
-        <v>29896000</v>
+        <v>40909000</v>
       </c>
       <c r="AJ9" s="55" t="s">
         <v>11</v>
       </c>
       <c r="AK9" s="63">
         <f>AC13</f>
-        <v>29896000</v>
+        <v>40909000</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -6944,14 +6932,14 @@
       </c>
       <c r="AC10" s="47">
         <f t="shared" si="0"/>
-        <v>32549932.89622917</v>
+        <v>42173848.818224415</v>
       </c>
       <c r="AE10" s="55" t="s">
         <v>12</v>
       </c>
       <c r="AF10" s="63">
         <f>AF9-AF8</f>
-        <v>20061190</v>
+        <v>31074190</v>
       </c>
       <c r="AJ10" s="55" t="s">
         <v>66</v>
@@ -7155,7 +7143,7 @@
       </c>
       <c r="AC12" s="24">
         <f t="shared" si="2"/>
-        <v>391098.81377083436</v>
+        <v>1780182.8917755932</v>
       </c>
       <c r="AE12" s="55" t="s">
         <v>17</v>
@@ -7169,7 +7157,7 @@
       </c>
       <c r="AK12" s="63">
         <f>AK9-(AK10-AK11)</f>
-        <v>29896000</v>
+        <v>40909000</v>
       </c>
     </row>
     <row r="13" spans="1:37">
@@ -7278,7 +7266,7 @@
         <v>21963184.870000001</v>
       </c>
       <c r="AC13" s="51">
-        <v>29896000</v>
+        <v>40909000</v>
       </c>
       <c r="AE13" s="55" t="s">
         <v>20</v>
@@ -7300,13 +7288,13 @@
       </c>
       <c r="AF15" s="63">
         <f>AF10*AF12</f>
-        <v>2530344.1037708297</v>
-      </c>
-      <c r="AI15" s="105" t="s">
+        <v>3919428.181775582</v>
+      </c>
+      <c r="AI15" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="AJ15" s="89"/>
-      <c r="AK15" s="89"/>
+      <c r="AJ15" s="95"/>
+      <c r="AK15" s="95"/>
     </row>
     <row r="16" spans="1:37">
       <c r="AE16" s="55" t="s">
@@ -7314,7 +7302,7 @@
       </c>
       <c r="AF16" s="63">
         <f>AF10*AF13</f>
-        <v>17530845.89622917</v>
+        <v>27154761.818224419</v>
       </c>
       <c r="AI16" s="55" t="s">
         <v>7</v>
@@ -7324,86 +7312,86 @@
       </c>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="91" t="s">
+      <c r="X17" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="92"/>
-      <c r="AA17" s="93"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="101"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="94" t="s">
+      <c r="X18" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="96"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="90"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="99"/>
-      <c r="Y19" s="100"/>
-      <c r="Z19" s="100"/>
-      <c r="AA19" s="101"/>
+      <c r="X19" s="91"/>
+      <c r="Y19" s="92"/>
+      <c r="Z19" s="92"/>
+      <c r="AA19" s="93"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="94" t="s">
+      <c r="X20" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="Y20" s="95"/>
-      <c r="Z20" s="95"/>
-      <c r="AA20" s="96"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="90"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="97"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="98"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="96"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="99"/>
-      <c r="Y22" s="100"/>
-      <c r="Z22" s="100"/>
-      <c r="AA22" s="101"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="93"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="94" t="s">
+      <c r="X23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="95"/>
-      <c r="Z23" s="95"/>
-      <c r="AA23" s="96"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="90"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="99"/>
-      <c r="Y24" s="100"/>
-      <c r="Z24" s="100"/>
-      <c r="AA24" s="101"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="92"/>
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="93"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="94" t="s">
+      <c r="X25" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="96"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="90"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="97"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="98"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="95"/>
+      <c r="Z27" s="95"/>
+      <c r="AA27" s="96"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="99"/>
-      <c r="Y28" s="100"/>
-      <c r="Z28" s="100"/>
-      <c r="AA28" s="101"/>
+      <c r="X28" s="91"/>
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="92"/>
+      <c r="AA28" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7428,7 +7416,7 @@
   <dimension ref="A1:AQ28"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH25" sqref="AH25"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -7461,15 +7449,15 @@
     </row>
     <row r="3" spans="1:43" ht="18" customHeight="1">
       <c r="A3" s="46"/>
-      <c r="AE3" s="90" t="s">
+      <c r="AE3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="89"/>
-      <c r="AI3" s="90" t="s">
+      <c r="AF3" s="95"/>
+      <c r="AI3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="89"/>
-      <c r="AK3" s="89"/>
+      <c r="AJ3" s="95"/>
+      <c r="AK3" s="95"/>
       <c r="AL3" s="6"/>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
@@ -7478,15 +7466,15 @@
       <c r="AQ3" s="6"/>
     </row>
     <row r="4" spans="1:43" ht="21" customHeight="1">
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AI4" s="106" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AI4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
       <c r="AL4" s="6"/>
       <c r="AM4" s="6"/>
       <c r="AQ4" s="6"/>
@@ -7882,14 +7870,14 @@
       </c>
       <c r="AF8" s="63">
         <f>AC13</f>
-        <v>97163000</v>
+        <v>101589000</v>
       </c>
       <c r="AJ8" s="55" t="s">
         <v>11</v>
       </c>
       <c r="AK8" s="63">
         <f>AC13</f>
-        <v>97163000</v>
+        <v>101589000</v>
       </c>
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
@@ -7985,7 +7973,7 @@
       </c>
       <c r="AC9" s="33">
         <f>AF15</f>
-        <v>27036674.876826026</v>
+        <v>29456220.471700188</v>
       </c>
       <c r="AD9" s="24"/>
       <c r="AE9" s="55" t="s">
@@ -7993,7 +7981,7 @@
       </c>
       <c r="AF9" s="63">
         <f>AF8-AF7</f>
-        <v>49457354</v>
+        <v>53883354</v>
       </c>
       <c r="AJ9" s="55" t="s">
         <v>66</v>
@@ -8120,7 +8108,7 @@
       </c>
       <c r="AC10" s="47">
         <f t="shared" si="0"/>
-        <v>101042855.87682602</v>
+        <v>103462401.47170019</v>
       </c>
       <c r="AD10" s="25"/>
       <c r="AE10" s="55"/>
@@ -8245,7 +8233,7 @@
       </c>
       <c r="AK11" s="63">
         <f>AK8-(AK9-AK10)</f>
-        <v>97163000</v>
+        <v>101589000</v>
       </c>
       <c r="AL11" s="6"/>
       <c r="AM11" s="6"/>
@@ -8348,7 +8336,7 @@
       </c>
       <c r="AC12" s="24">
         <f t="shared" si="2"/>
-        <v>14851547.073173985</v>
+        <v>16858001.478299811</v>
       </c>
       <c r="AD12" s="24"/>
       <c r="AE12" s="55" t="s">
@@ -8471,7 +8459,7 @@
         <v>86621053.290000007</v>
       </c>
       <c r="AC13" s="51">
-        <v>97163000</v>
+        <v>101589000</v>
       </c>
       <c r="AD13" s="25"/>
       <c r="AE13" s="55"/>
@@ -8485,13 +8473,13 @@
       </c>
       <c r="AF14" s="63">
         <f>AF9*AF11</f>
-        <v>22420679.123173971</v>
-      </c>
-      <c r="AI14" s="105" t="s">
+        <v>24427133.528299809</v>
+      </c>
+      <c r="AI14" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="AJ14" s="89"/>
-      <c r="AK14" s="89"/>
+      <c r="AJ14" s="95"/>
+      <c r="AK14" s="95"/>
     </row>
     <row r="15" spans="1:43">
       <c r="AE15" s="55" t="s">
@@ -8499,7 +8487,7 @@
       </c>
       <c r="AF15" s="63">
         <f>AF9*AF12</f>
-        <v>27036674.876826026</v>
+        <v>29456220.471700188</v>
       </c>
       <c r="AI15" s="55" t="s">
         <v>7</v>
@@ -8509,86 +8497,86 @@
       </c>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="91" t="s">
+      <c r="X17" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="92"/>
-      <c r="AA17" s="93"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="101"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="94" t="s">
+      <c r="X18" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="96"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="90"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="99"/>
-      <c r="Y19" s="100"/>
-      <c r="Z19" s="100"/>
-      <c r="AA19" s="101"/>
+      <c r="X19" s="91"/>
+      <c r="Y19" s="92"/>
+      <c r="Z19" s="92"/>
+      <c r="AA19" s="93"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="94" t="s">
+      <c r="X20" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="Y20" s="95"/>
-      <c r="Z20" s="95"/>
-      <c r="AA20" s="96"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="90"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="97"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="98"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="96"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="99"/>
-      <c r="Y22" s="100"/>
-      <c r="Z22" s="100"/>
-      <c r="AA22" s="101"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="93"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="94" t="s">
+      <c r="X23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="95"/>
-      <c r="Z23" s="95"/>
-      <c r="AA23" s="96"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="90"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="99"/>
-      <c r="Y24" s="100"/>
-      <c r="Z24" s="100"/>
-      <c r="AA24" s="101"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="92"/>
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="93"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="94" t="s">
+      <c r="X25" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="96"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="90"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="97"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="98"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="95"/>
+      <c r="Z27" s="95"/>
+      <c r="AA27" s="96"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="99"/>
-      <c r="Y28" s="100"/>
-      <c r="Z28" s="100"/>
-      <c r="AA28" s="101"/>
+      <c r="X28" s="91"/>
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="92"/>
+      <c r="AA28" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -8612,7 +8600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
@@ -8651,18 +8639,18 @@
     </row>
     <row r="4" spans="1:44" ht="21" customHeight="1">
       <c r="A4" s="19"/>
-      <c r="AE4" s="90" t="s">
+      <c r="AE4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="89"/>
-      <c r="AH4" s="90" t="s">
+      <c r="AF4" s="95"/>
+      <c r="AH4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="89"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
       <c r="AK4" s="108"/>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="95"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="6"/>
     </row>
@@ -8753,12 +8741,12 @@
         <v>2023</v>
       </c>
       <c r="AD5" s="83"/>
-      <c r="AE5" s="88" t="s">
+      <c r="AE5" s="97" t="s">
         <v>5</v>
       </c>
       <c r="AF5" s="107"/>
       <c r="AG5" s="83"/>
-      <c r="AH5" s="106" t="s">
+      <c r="AH5" s="105" t="s">
         <v>6</v>
       </c>
       <c r="AI5" s="107"/>
@@ -9167,7 +9155,7 @@
       </c>
       <c r="AC9" s="18">
         <f>AF16</f>
-        <v>6880669.3081125207</v>
+        <v>6431587.2317887843</v>
       </c>
       <c r="AD9" s="24"/>
       <c r="AE9" s="55" t="s">
@@ -9175,7 +9163,7 @@
       </c>
       <c r="AF9" s="63">
         <f>AC13</f>
-        <v>33128000</v>
+        <v>32315000</v>
       </c>
       <c r="AG9" s="24"/>
       <c r="AI9" s="55" t="s">
@@ -9308,7 +9296,7 @@
       </c>
       <c r="AC10" s="25">
         <f t="shared" si="0"/>
-        <v>33635976.308112517</v>
+        <v>33186894.231788784</v>
       </c>
       <c r="AD10" s="25"/>
       <c r="AE10" s="55" t="s">
@@ -9316,7 +9304,7 @@
       </c>
       <c r="AF10" s="63">
         <f>AF9-AF8</f>
-        <v>12456485</v>
+        <v>11643485</v>
       </c>
       <c r="AG10" s="25"/>
       <c r="AI10" s="55" t="s">
@@ -9537,7 +9525,7 @@
       </c>
       <c r="AC12" s="24">
         <f t="shared" si="2"/>
-        <v>2455194.5518874824</v>
+        <v>2091276.6282112151</v>
       </c>
       <c r="AD12" s="24"/>
       <c r="AE12" s="55" t="s">
@@ -9662,7 +9650,7 @@
         <v>26054690.649999999</v>
       </c>
       <c r="AC13" s="51">
-        <v>33128000</v>
+        <v>32315000</v>
       </c>
       <c r="AD13" s="25"/>
       <c r="AE13" s="55" t="s">
@@ -9674,8 +9662,8 @@
       </c>
       <c r="AG13" s="25"/>
       <c r="AK13" s="109"/>
-      <c r="AL13" s="89"/>
-      <c r="AM13" s="89"/>
+      <c r="AL13" s="95"/>
+      <c r="AM13" s="95"/>
     </row>
     <row r="14" spans="1:44">
       <c r="A14" s="19"/>
@@ -9693,13 +9681,13 @@
       </c>
       <c r="AF15" s="63">
         <f>AF10*AF12</f>
-        <v>5575815.6918874793</v>
-      </c>
-      <c r="AH15" s="105" t="s">
+        <v>5211897.7682112157</v>
+      </c>
+      <c r="AH15" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="AI15" s="89"/>
-      <c r="AJ15" s="89"/>
+      <c r="AI15" s="95"/>
+      <c r="AJ15" s="95"/>
     </row>
     <row r="16" spans="1:44">
       <c r="AE16" s="55" t="s">
@@ -9707,7 +9695,7 @@
       </c>
       <c r="AF16" s="63">
         <f>AF10*AF13</f>
-        <v>6880669.3081125207</v>
+        <v>6431587.2317887843</v>
       </c>
       <c r="AH16" s="55" t="s">
         <v>7</v>
@@ -9717,86 +9705,86 @@
       </c>
     </row>
     <row r="17" spans="24:27" ht="21" customHeight="1">
-      <c r="X17" s="91" t="s">
+      <c r="X17" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="92"/>
-      <c r="AA17" s="93"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="101"/>
     </row>
     <row r="18" spans="24:27">
-      <c r="X18" s="94" t="s">
+      <c r="X18" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="96"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="90"/>
     </row>
     <row r="19" spans="24:27">
-      <c r="X19" s="99"/>
-      <c r="Y19" s="100"/>
-      <c r="Z19" s="100"/>
-      <c r="AA19" s="101"/>
+      <c r="X19" s="91"/>
+      <c r="Y19" s="92"/>
+      <c r="Z19" s="92"/>
+      <c r="AA19" s="93"/>
     </row>
     <row r="20" spans="24:27">
-      <c r="X20" s="94" t="s">
+      <c r="X20" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="Y20" s="95"/>
-      <c r="Z20" s="95"/>
-      <c r="AA20" s="96"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="90"/>
     </row>
     <row r="21" spans="24:27">
-      <c r="X21" s="97"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="98"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="96"/>
     </row>
     <row r="22" spans="24:27">
-      <c r="X22" s="99"/>
-      <c r="Y22" s="100"/>
-      <c r="Z22" s="100"/>
-      <c r="AA22" s="101"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="93"/>
     </row>
     <row r="23" spans="24:27">
-      <c r="X23" s="94" t="s">
+      <c r="X23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="95"/>
-      <c r="Z23" s="95"/>
-      <c r="AA23" s="96"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="90"/>
     </row>
     <row r="24" spans="24:27">
-      <c r="X24" s="99"/>
-      <c r="Y24" s="100"/>
-      <c r="Z24" s="100"/>
-      <c r="AA24" s="101"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="92"/>
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="93"/>
     </row>
     <row r="25" spans="24:27">
-      <c r="X25" s="94" t="s">
+      <c r="X25" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="96"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="90"/>
     </row>
     <row r="26" spans="24:27">
-      <c r="X26" s="97"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="98"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="96"/>
     </row>
     <row r="27" spans="24:27">
-      <c r="X27" s="97"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="98"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="95"/>
+      <c r="Z27" s="95"/>
+      <c r="AA27" s="96"/>
     </row>
     <row r="28" spans="24:27">
-      <c r="X28" s="99"/>
-      <c r="Y28" s="100"/>
-      <c r="Z28" s="100"/>
-      <c r="AA28" s="101"/>
+      <c r="X28" s="91"/>
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="92"/>
+      <c r="AA28" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -9822,8 +9810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
@@ -9856,15 +9844,15 @@
     </row>
     <row r="4" spans="1:17" ht="21" customHeight="1">
       <c r="A4" s="19"/>
-      <c r="J4" s="90" t="s">
+      <c r="J4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="89"/>
-      <c r="M4" s="90" t="s">
+      <c r="K4" s="95"/>
+      <c r="M4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
     </row>
     <row r="5" spans="1:17" s="19" customFormat="1" ht="21" customHeight="1">
       <c r="A5" s="21"/>
@@ -9889,12 +9877,12 @@
       <c r="H5" s="11">
         <v>2023</v>
       </c>
-      <c r="J5" s="88" t="s">
+      <c r="J5" s="97" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="107"/>
       <c r="L5" s="83"/>
-      <c r="M5" s="106" t="s">
+      <c r="M5" s="105" t="s">
         <v>6</v>
       </c>
       <c r="N5" s="107"/>
@@ -10025,14 +10013,14 @@
       </c>
       <c r="H9" s="18">
         <f>K16</f>
-        <v>16726420.571576921</v>
+        <v>19076755.134599701</v>
       </c>
       <c r="J9" s="55" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="63">
         <f>H13</f>
-        <v>68087000</v>
+        <v>72594000</v>
       </c>
       <c r="L9" s="24"/>
       <c r="N9" s="55" t="s">
@@ -10075,14 +10063,14 @@
       </c>
       <c r="H10" s="25">
         <f t="shared" si="0"/>
-        <v>71241253.571576923</v>
+        <v>73591588.134599701</v>
       </c>
       <c r="J10" s="55" t="s">
         <v>12</v>
       </c>
       <c r="K10" s="63">
         <f>K9-K8</f>
-        <v>32074573</v>
+        <v>36581573</v>
       </c>
       <c r="L10" s="25"/>
       <c r="N10" s="55" t="s">
@@ -10163,7 +10151,7 @@
       </c>
       <c r="H12" s="24">
         <f t="shared" si="2"/>
-        <v>3084342.5084230751</v>
+        <v>5241007.9454002976</v>
       </c>
       <c r="J12" s="55" t="s">
         <v>17</v>
@@ -10204,7 +10192,7 @@
         <v>75366810.969999999</v>
       </c>
       <c r="H13" s="51">
-        <v>68087000</v>
+        <v>72594000</v>
       </c>
       <c r="J13" s="55" t="s">
         <v>20</v>
@@ -10228,13 +10216,13 @@
       </c>
       <c r="K15" s="63">
         <f>K10*K12</f>
-        <v>15348152.428423077</v>
-      </c>
-      <c r="M15" s="105" t="s">
+        <v>17504817.865400299</v>
+      </c>
+      <c r="M15" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
     </row>
     <row r="16" spans="1:17">
       <c r="J16" s="55" t="s">
@@ -10242,7 +10230,7 @@
       </c>
       <c r="K16" s="63">
         <f>K10*K13</f>
-        <v>16726420.571576921</v>
+        <v>19076755.134599701</v>
       </c>
       <c r="M16" s="55" t="s">
         <v>7</v>
@@ -10252,86 +10240,86 @@
       </c>
     </row>
     <row r="17" spans="3:6" ht="21" customHeight="1">
-      <c r="C17" s="91" t="s">
+      <c r="C17" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="93"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="101"/>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="94" t="s">
+      <c r="C18" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="96"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="99"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="101"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="93"/>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="94" t="s">
+      <c r="C20" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="96"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="90"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="97"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="98"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="96"/>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="99"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="101"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="93"/>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="94" t="s">
+      <c r="C23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="96"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="90"/>
     </row>
     <row r="24" spans="3:6">
-      <c r="C24" s="99"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="101"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="93"/>
     </row>
     <row r="25" spans="3:6">
-      <c r="C25" s="94" t="s">
+      <c r="C25" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="96"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="90"/>
     </row>
     <row r="26" spans="3:6">
-      <c r="C26" s="97"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="98"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="96"/>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="97"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="98"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="96"/>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="99"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="101"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -10378,10 +10366,10 @@
       <c r="G1" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="101"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="72" t="s">
@@ -10396,10 +10384,10 @@
       <c r="G3" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="101"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="93"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="19" t="s">

</xml_diff>